<commit_message>
Update Aganda, scheduled future tasks and add '.gitnore' file.
</commit_message>
<xml_diff>
--- a/MainAgenda.xlsx
+++ b/MainAgenda.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0063C04C-EDFE-44DA-A534-23084B25EEDF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D4DF1E09-830E-4307-8BF1-3B6613F472A2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="总体计划草图" sheetId="1" r:id="rId1"/>
     <sheet name="V0.1.0开发计划" sheetId="3" r:id="rId2"/>
-    <sheet name="功能" sheetId="2" r:id="rId3"/>
+    <sheet name="交付物" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,10 +72,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>~</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -104,15 +100,99 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>画用户界面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>画UML用例图</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>定义每个任务预计开始和结束时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发布V0.1.0版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分析完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总体测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定义组件之间的接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计网站总体框架（MVC）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定义流程算法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计各个组件的关联和边界</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>画网页界面原型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定义类图，活动图，状态机图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>制作逻辑层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>制作网页的静态部分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>制作视图层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单元测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分析阶段：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UML场景描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UML用例图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>界面原型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -120,7 +200,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,8 +232,27 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,8 +287,13 @@
         <fgColor theme="8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -206,8 +310,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -218,8 +331,11 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -231,11 +347,22 @@
     <xf numFmtId="58" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="标题 2" xfId="1" builtinId="17"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="着色 2" xfId="2" builtinId="33"/>
+    <cellStyle name="着色 3" xfId="4" builtinId="37"/>
     <cellStyle name="着色 5" xfId="3" builtinId="45"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -525,7 +652,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -604,22 +731,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC988E25-B343-4608-AF8D-463AF7A5B44B}">
-  <dimension ref="A1:V11"/>
+  <dimension ref="A1:Y180"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.75" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
     <col min="15" max="15" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.6640625" customWidth="1"/>
+    <col min="25" max="25" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="5">
         <v>43199</v>
@@ -684,67 +816,1640 @@
       <c r="V1" s="5">
         <v>43219</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="W1" s="5">
+        <v>43220</v>
+      </c>
+      <c r="X1" s="5">
+        <v>43221</v>
+      </c>
+      <c r="Y1" s="5">
+        <v>43222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="14"/>
+      <c r="O3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="14"/>
+      <c r="W3" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y3" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="10"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="W4" s="10"/>
+      <c r="Y4" s="10"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="7"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="H5" s="10"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="10"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="W5" s="10"/>
+      <c r="Y5" s="10"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="E6" s="7"/>
+      <c r="H6" s="10"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="10"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="W6" s="10"/>
+      <c r="Y6" s="10"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="E7" s="7"/>
+      <c r="H7" s="10"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="10"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="W7" s="10"/>
+      <c r="Y7" s="10"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="E8" s="7"/>
+      <c r="H8" s="10"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="10"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="W8" s="10"/>
+      <c r="Y8" s="10"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="E9" s="7"/>
+      <c r="H9" s="10"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="10"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="W9" s="10"/>
+      <c r="Y9" s="10"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="H10" s="10"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="10"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="W10" s="10"/>
+      <c r="Y10" s="10"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="H11" s="10"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="10"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="W11" s="10"/>
+      <c r="Y11" s="10"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="G12" s="8"/>
+      <c r="H12" s="11"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="10"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="W12" s="10"/>
+      <c r="Y12" s="10"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="10"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="W13" s="10"/>
+      <c r="Y13" s="10"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="8"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="W14" s="10"/>
+      <c r="Y14" s="10"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="J15" s="8"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="W15" s="10"/>
+      <c r="Y15" s="10"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="W16" s="10"/>
+      <c r="Y16" s="10"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
+      <c r="W17" s="10"/>
+      <c r="Y17" s="10"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="W18" s="10"/>
+      <c r="Y18" s="10"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="H19" s="10"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="12"/>
+      <c r="Y19" s="10"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="10"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="W20" s="10"/>
+      <c r="Y20" s="10"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="10"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="10"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="16"/>
+      <c r="U21" s="14"/>
+      <c r="W21" s="10"/>
+      <c r="Y21" s="10"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" s="10"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="10"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="14"/>
+      <c r="W22" s="10"/>
+      <c r="Y22" s="10"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="10"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="10"/>
+      <c r="T23" s="14"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="11"/>
+      <c r="Y23" s="10"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="10"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="10"/>
+      <c r="T24" s="14"/>
+      <c r="U24" s="14"/>
+      <c r="W24" s="11"/>
+      <c r="Y24" s="10"/>
+    </row>
+    <row r="25" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="10"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="10"/>
+      <c r="T25" s="14"/>
+      <c r="U25" s="14"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="12"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="H26" s="10"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="T26" s="14"/>
+      <c r="U26" s="14"/>
+      <c r="W26" s="10"/>
+      <c r="Y26" s="10"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="H27" s="10"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="14"/>
+      <c r="S27" s="14"/>
+      <c r="T27" s="14"/>
+      <c r="W27" s="10"/>
+      <c r="Y27" s="10"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="H28" s="10"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="14"/>
+      <c r="S28" s="14"/>
+      <c r="T28" s="14"/>
+      <c r="W28" s="10"/>
+      <c r="Y28" s="10"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="H29" s="10"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="14"/>
+      <c r="S29" s="14"/>
+      <c r="T29" s="14"/>
+      <c r="W29" s="10"/>
+      <c r="Y29" s="10"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="H30" s="10"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="14"/>
+      <c r="S30" s="14"/>
+      <c r="T30" s="14"/>
+      <c r="W30" s="10"/>
+      <c r="Y30" s="10"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="H31" s="10"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="14"/>
+      <c r="S31" s="14"/>
+      <c r="T31" s="14"/>
+      <c r="W31" s="10"/>
+      <c r="Y31" s="10"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="H32" s="10"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="14"/>
+      <c r="S32" s="14"/>
+      <c r="T32" s="14"/>
+      <c r="W32" s="10"/>
+      <c r="Y32" s="10"/>
+    </row>
+    <row r="33" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H33" s="10"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="14"/>
+      <c r="S33" s="14"/>
+      <c r="T33" s="14"/>
+      <c r="W33" s="10"/>
+      <c r="Y33" s="10"/>
+    </row>
+    <row r="34" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H34" s="10"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="14"/>
+      <c r="S34" s="14"/>
+      <c r="T34" s="14"/>
+      <c r="W34" s="10"/>
+      <c r="Y34" s="10"/>
+    </row>
+    <row r="35" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H35" s="10"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="14"/>
+      <c r="S35" s="14"/>
+      <c r="T35" s="14"/>
+      <c r="W35" s="10"/>
+      <c r="Y35" s="10"/>
+    </row>
+    <row r="36" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H36" s="10"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="14"/>
+      <c r="S36" s="14"/>
+      <c r="T36" s="14"/>
+      <c r="W36" s="10"/>
+      <c r="Y36" s="10"/>
+    </row>
+    <row r="37" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H37" s="10"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="14"/>
+      <c r="W37" s="10"/>
+      <c r="Y37" s="10"/>
+    </row>
+    <row r="38" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H38" s="10"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="14"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="14"/>
+      <c r="W38" s="10"/>
+      <c r="Y38" s="10"/>
+    </row>
+    <row r="39" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H39" s="10"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="14"/>
+      <c r="S39" s="14"/>
+      <c r="T39" s="14"/>
+      <c r="W39" s="10"/>
+      <c r="Y39" s="10"/>
+    </row>
+    <row r="40" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H40" s="10"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="14"/>
+      <c r="S40" s="14"/>
+      <c r="T40" s="14"/>
+      <c r="W40" s="10"/>
+      <c r="Y40" s="10"/>
+    </row>
+    <row r="41" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H41" s="10"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="14"/>
+      <c r="S41" s="14"/>
+      <c r="T41" s="14"/>
+      <c r="W41" s="10"/>
+      <c r="Y41" s="10"/>
+    </row>
+    <row r="42" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H42" s="10"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="14"/>
+      <c r="W42" s="10"/>
+      <c r="Y42" s="10"/>
+    </row>
+    <row r="43" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H43" s="10"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="14"/>
+      <c r="S43" s="14"/>
+      <c r="T43" s="14"/>
+      <c r="W43" s="10"/>
+      <c r="Y43" s="10"/>
+    </row>
+    <row r="44" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H44" s="10"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="14"/>
+      <c r="S44" s="14"/>
+      <c r="T44" s="14"/>
+      <c r="W44" s="10"/>
+      <c r="Y44" s="10"/>
+    </row>
+    <row r="45" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H45" s="10"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="14"/>
+      <c r="S45" s="14"/>
+      <c r="T45" s="14"/>
+      <c r="W45" s="10"/>
+      <c r="Y45" s="10"/>
+    </row>
+    <row r="46" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H46" s="10"/>
+      <c r="M46" s="14"/>
+      <c r="N46" s="14"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="14"/>
+      <c r="S46" s="14"/>
+      <c r="T46" s="14"/>
+      <c r="W46" s="10"/>
+      <c r="Y46" s="10"/>
+    </row>
+    <row r="47" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H47" s="10"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="14"/>
+      <c r="S47" s="14"/>
+      <c r="T47" s="14"/>
+      <c r="W47" s="10"/>
+      <c r="Y47" s="10"/>
+    </row>
+    <row r="48" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H48" s="10"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="14"/>
+      <c r="S48" s="14"/>
+      <c r="T48" s="14"/>
+      <c r="W48" s="10"/>
+      <c r="Y48" s="10"/>
+    </row>
+    <row r="49" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H49" s="10"/>
+      <c r="M49" s="14"/>
+      <c r="N49" s="14"/>
+      <c r="O49" s="10"/>
+      <c r="P49" s="14"/>
+      <c r="S49" s="14"/>
+      <c r="T49" s="14"/>
+      <c r="W49" s="10"/>
+      <c r="Y49" s="10"/>
+    </row>
+    <row r="50" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H50" s="10"/>
+      <c r="M50" s="14"/>
+      <c r="N50" s="14"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="14"/>
+      <c r="S50" s="14"/>
+      <c r="T50" s="14"/>
+      <c r="W50" s="10"/>
+      <c r="Y50" s="10"/>
+    </row>
+    <row r="51" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H51" s="10"/>
+      <c r="M51" s="14"/>
+      <c r="N51" s="14"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="14"/>
+      <c r="S51" s="14"/>
+      <c r="T51" s="14"/>
+      <c r="W51" s="10"/>
+      <c r="Y51" s="10"/>
+    </row>
+    <row r="52" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H52" s="10"/>
+      <c r="M52" s="14"/>
+      <c r="N52" s="14"/>
+      <c r="O52" s="10"/>
+      <c r="P52" s="14"/>
+      <c r="S52" s="14"/>
+      <c r="T52" s="14"/>
+      <c r="W52" s="10"/>
+      <c r="Y52" s="10"/>
+    </row>
+    <row r="53" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H53" s="10"/>
+      <c r="M53" s="14"/>
+      <c r="N53" s="14"/>
+      <c r="O53" s="10"/>
+      <c r="P53" s="14"/>
+      <c r="S53" s="14"/>
+      <c r="T53" s="14"/>
+      <c r="W53" s="10"/>
+      <c r="Y53" s="10"/>
+    </row>
+    <row r="54" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H54" s="10"/>
+      <c r="M54" s="14"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="10"/>
+      <c r="P54" s="14"/>
+      <c r="S54" s="14"/>
+      <c r="T54" s="14"/>
+      <c r="W54" s="10"/>
+      <c r="Y54" s="10"/>
+    </row>
+    <row r="55" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H55" s="10"/>
+      <c r="M55" s="14"/>
+      <c r="N55" s="14"/>
+      <c r="O55" s="10"/>
+      <c r="P55" s="14"/>
+      <c r="S55" s="14"/>
+      <c r="T55" s="14"/>
+      <c r="W55" s="10"/>
+      <c r="Y55" s="10"/>
+    </row>
+    <row r="56" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H56" s="10"/>
+      <c r="M56" s="14"/>
+      <c r="N56" s="14"/>
+      <c r="O56" s="10"/>
+      <c r="P56" s="14"/>
+      <c r="S56" s="14"/>
+      <c r="T56" s="14"/>
+      <c r="W56" s="10"/>
+      <c r="Y56" s="10"/>
+    </row>
+    <row r="57" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H57" s="10"/>
+      <c r="M57" s="14"/>
+      <c r="N57" s="14"/>
+      <c r="O57" s="10"/>
+      <c r="P57" s="14"/>
+      <c r="S57" s="14"/>
+      <c r="T57" s="14"/>
+      <c r="W57" s="10"/>
+      <c r="Y57" s="10"/>
+    </row>
+    <row r="58" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H58" s="10"/>
+      <c r="M58" s="14"/>
+      <c r="N58" s="14"/>
+      <c r="O58" s="10"/>
+      <c r="P58" s="14"/>
+      <c r="S58" s="14"/>
+      <c r="T58" s="14"/>
+      <c r="W58" s="10"/>
+      <c r="Y58" s="10"/>
+    </row>
+    <row r="59" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H59" s="10"/>
+      <c r="M59" s="14"/>
+      <c r="N59" s="14"/>
+      <c r="O59" s="10"/>
+      <c r="P59" s="14"/>
+      <c r="S59" s="14"/>
+      <c r="T59" s="14"/>
+      <c r="W59" s="10"/>
+      <c r="Y59" s="10"/>
+    </row>
+    <row r="60" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H60" s="10"/>
+      <c r="M60" s="14"/>
+      <c r="N60" s="14"/>
+      <c r="O60" s="10"/>
+      <c r="P60" s="14"/>
+      <c r="S60" s="14"/>
+      <c r="T60" s="14"/>
+      <c r="W60" s="10"/>
+      <c r="Y60" s="10"/>
+    </row>
+    <row r="61" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H61" s="10"/>
+      <c r="M61" s="14"/>
+      <c r="N61" s="14"/>
+      <c r="O61" s="10"/>
+      <c r="P61" s="14"/>
+      <c r="S61" s="14"/>
+      <c r="T61" s="14"/>
+      <c r="W61" s="10"/>
+      <c r="Y61" s="10"/>
+    </row>
+    <row r="62" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H62" s="10"/>
+      <c r="M62" s="14"/>
+      <c r="N62" s="14"/>
+      <c r="O62" s="10"/>
+      <c r="P62" s="14"/>
+      <c r="S62" s="14"/>
+      <c r="T62" s="14"/>
+      <c r="W62" s="10"/>
+      <c r="Y62" s="10"/>
+    </row>
+    <row r="63" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H63" s="10"/>
+      <c r="M63" s="14"/>
+      <c r="N63" s="14"/>
+      <c r="O63" s="10"/>
+      <c r="P63" s="14"/>
+      <c r="S63" s="14"/>
+      <c r="T63" s="14"/>
+      <c r="W63" s="10"/>
+      <c r="Y63" s="10"/>
+    </row>
+    <row r="64" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H64" s="10"/>
+      <c r="M64" s="14"/>
+      <c r="N64" s="14"/>
+      <c r="O64" s="10"/>
+      <c r="P64" s="14"/>
+      <c r="S64" s="14"/>
+      <c r="T64" s="14"/>
+      <c r="W64" s="10"/>
+      <c r="Y64" s="10"/>
+    </row>
+    <row r="65" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H65" s="10"/>
+      <c r="M65" s="14"/>
+      <c r="N65" s="14"/>
+      <c r="O65" s="10"/>
+      <c r="P65" s="14"/>
+      <c r="S65" s="14"/>
+      <c r="T65" s="14"/>
+      <c r="W65" s="10"/>
+      <c r="Y65" s="10"/>
+    </row>
+    <row r="66" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H66" s="10"/>
+      <c r="M66" s="14"/>
+      <c r="N66" s="14"/>
+      <c r="O66" s="10"/>
+      <c r="P66" s="14"/>
+      <c r="S66" s="14"/>
+      <c r="T66" s="14"/>
+      <c r="W66" s="10"/>
+      <c r="Y66" s="10"/>
+    </row>
+    <row r="67" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H67" s="10"/>
+      <c r="M67" s="14"/>
+      <c r="N67" s="14"/>
+      <c r="O67" s="10"/>
+      <c r="P67" s="14"/>
+      <c r="S67" s="14"/>
+      <c r="T67" s="14"/>
+      <c r="W67" s="10"/>
+      <c r="Y67" s="10"/>
+    </row>
+    <row r="68" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H68" s="10"/>
+      <c r="M68" s="14"/>
+      <c r="N68" s="14"/>
+      <c r="O68" s="10"/>
+      <c r="P68" s="14"/>
+      <c r="S68" s="14"/>
+      <c r="T68" s="14"/>
+      <c r="W68" s="10"/>
+      <c r="Y68" s="10"/>
+    </row>
+    <row r="69" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H69" s="10"/>
+      <c r="M69" s="14"/>
+      <c r="N69" s="14"/>
+      <c r="O69" s="10"/>
+      <c r="P69" s="14"/>
+      <c r="S69" s="14"/>
+      <c r="T69" s="14"/>
+      <c r="W69" s="10"/>
+      <c r="Y69" s="10"/>
+    </row>
+    <row r="70" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="H70" s="10"/>
+      <c r="M70" s="14"/>
+      <c r="N70" s="14"/>
+      <c r="O70" s="10"/>
+      <c r="P70" s="14"/>
+      <c r="S70" s="14"/>
+      <c r="T70" s="14"/>
+      <c r="W70" s="10"/>
+      <c r="Y70" s="10"/>
+    </row>
+    <row r="71" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="M71" s="14"/>
+      <c r="N71" s="14"/>
+      <c r="O71" s="14"/>
+      <c r="P71" s="14"/>
+      <c r="S71" s="14"/>
+      <c r="T71" s="14"/>
+    </row>
+    <row r="72" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="M72" s="14"/>
+      <c r="N72" s="14"/>
+      <c r="O72" s="14"/>
+      <c r="P72" s="14"/>
+      <c r="S72" s="14"/>
+      <c r="T72" s="14"/>
+    </row>
+    <row r="73" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="M73" s="14"/>
+      <c r="N73" s="14"/>
+      <c r="O73" s="14"/>
+      <c r="P73" s="14"/>
+      <c r="S73" s="14"/>
+      <c r="T73" s="14"/>
+    </row>
+    <row r="74" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="M74" s="14"/>
+      <c r="N74" s="14"/>
+      <c r="O74" s="14"/>
+      <c r="P74" s="14"/>
+      <c r="S74" s="14"/>
+      <c r="T74" s="14"/>
+      <c r="Y74" s="14"/>
+    </row>
+    <row r="75" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="M75" s="14"/>
+      <c r="N75" s="14"/>
+      <c r="O75" s="14"/>
+      <c r="P75" s="14"/>
+      <c r="S75" s="14"/>
+      <c r="T75" s="14"/>
+    </row>
+    <row r="76" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="M76" s="14"/>
+      <c r="N76" s="14"/>
+      <c r="O76" s="14"/>
+      <c r="P76" s="14"/>
+      <c r="S76" s="14"/>
+      <c r="T76" s="14"/>
+    </row>
+    <row r="77" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="M77" s="14"/>
+      <c r="N77" s="14"/>
+      <c r="O77" s="14"/>
+      <c r="P77" s="14"/>
+      <c r="S77" s="14"/>
+      <c r="T77" s="14"/>
+    </row>
+    <row r="78" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="M78" s="14"/>
+      <c r="N78" s="14"/>
+      <c r="O78" s="14"/>
+      <c r="P78" s="14"/>
+      <c r="S78" s="14"/>
+      <c r="T78" s="14"/>
+    </row>
+    <row r="79" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="M79" s="14"/>
+      <c r="N79" s="14"/>
+      <c r="O79" s="14"/>
+      <c r="P79" s="14"/>
+      <c r="S79" s="14"/>
+      <c r="T79" s="14"/>
+    </row>
+    <row r="80" spans="8:25" x14ac:dyDescent="0.3">
+      <c r="M80" s="14"/>
+      <c r="N80" s="14"/>
+      <c r="O80" s="14"/>
+      <c r="P80" s="14"/>
+      <c r="S80" s="14"/>
+      <c r="T80" s="14"/>
+    </row>
+    <row r="81" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M81" s="14"/>
+      <c r="N81" s="14"/>
+      <c r="O81" s="14"/>
+      <c r="P81" s="14"/>
+      <c r="S81" s="14"/>
+      <c r="T81" s="14"/>
+    </row>
+    <row r="82" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M82" s="14"/>
+      <c r="N82" s="14"/>
+      <c r="O82" s="14"/>
+      <c r="P82" s="14"/>
+      <c r="S82" s="14"/>
+      <c r="T82" s="14"/>
+    </row>
+    <row r="83" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M83" s="14"/>
+      <c r="N83" s="14"/>
+      <c r="O83" s="14"/>
+      <c r="P83" s="14"/>
+      <c r="S83" s="14"/>
+      <c r="T83" s="14"/>
+    </row>
+    <row r="84" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M84" s="14"/>
+      <c r="N84" s="14"/>
+      <c r="O84" s="14"/>
+      <c r="P84" s="14"/>
+      <c r="S84" s="14"/>
+      <c r="T84" s="14"/>
+    </row>
+    <row r="85" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M85" s="14"/>
+      <c r="N85" s="14"/>
+      <c r="O85" s="14"/>
+      <c r="P85" s="14"/>
+      <c r="S85" s="14"/>
+      <c r="T85" s="14"/>
+    </row>
+    <row r="86" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M86" s="14"/>
+      <c r="N86" s="14"/>
+      <c r="O86" s="14"/>
+      <c r="P86" s="14"/>
+      <c r="S86" s="14"/>
+      <c r="T86" s="14"/>
+    </row>
+    <row r="87" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M87" s="14"/>
+      <c r="N87" s="14"/>
+      <c r="O87" s="14"/>
+      <c r="P87" s="14"/>
+      <c r="S87" s="14"/>
+      <c r="T87" s="14"/>
+    </row>
+    <row r="88" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M88" s="14"/>
+      <c r="N88" s="14"/>
+      <c r="O88" s="14"/>
+      <c r="P88" s="14"/>
+      <c r="S88" s="14"/>
+      <c r="T88" s="14"/>
+    </row>
+    <row r="89" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M89" s="14"/>
+      <c r="N89" s="14"/>
+      <c r="O89" s="14"/>
+      <c r="P89" s="14"/>
+      <c r="S89" s="14"/>
+      <c r="T89" s="14"/>
+    </row>
+    <row r="90" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M90" s="14"/>
+      <c r="N90" s="14"/>
+      <c r="O90" s="14"/>
+      <c r="P90" s="14"/>
+      <c r="S90" s="14"/>
+      <c r="T90" s="14"/>
+    </row>
+    <row r="91" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M91" s="14"/>
+      <c r="N91" s="14"/>
+      <c r="O91" s="14"/>
+      <c r="P91" s="14"/>
+      <c r="S91" s="14"/>
+      <c r="T91" s="14"/>
+    </row>
+    <row r="92" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M92" s="14"/>
+      <c r="N92" s="14"/>
+      <c r="O92" s="14"/>
+      <c r="P92" s="14"/>
+      <c r="S92" s="14"/>
+      <c r="T92" s="14"/>
+    </row>
+    <row r="93" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M93" s="14"/>
+      <c r="N93" s="14"/>
+      <c r="O93" s="14"/>
+      <c r="P93" s="14"/>
+      <c r="S93" s="14"/>
+      <c r="T93" s="14"/>
+    </row>
+    <row r="94" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M94" s="14"/>
+      <c r="N94" s="14"/>
+      <c r="O94" s="14"/>
+      <c r="P94" s="14"/>
+      <c r="S94" s="14"/>
+      <c r="T94" s="14"/>
+    </row>
+    <row r="95" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M95" s="14"/>
+      <c r="N95" s="14"/>
+      <c r="O95" s="14"/>
+      <c r="P95" s="14"/>
+      <c r="S95" s="14"/>
+      <c r="T95" s="14"/>
+    </row>
+    <row r="96" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M96" s="14"/>
+      <c r="N96" s="14"/>
+      <c r="O96" s="14"/>
+      <c r="P96" s="14"/>
+      <c r="S96" s="14"/>
+      <c r="T96" s="14"/>
+    </row>
+    <row r="97" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M97" s="14"/>
+      <c r="N97" s="14"/>
+      <c r="O97" s="14"/>
+      <c r="P97" s="14"/>
+      <c r="S97" s="14"/>
+      <c r="T97" s="14"/>
+    </row>
+    <row r="98" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M98" s="14"/>
+      <c r="N98" s="14"/>
+      <c r="O98" s="14"/>
+      <c r="P98" s="14"/>
+      <c r="S98" s="14"/>
+      <c r="T98" s="14"/>
+    </row>
+    <row r="99" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M99" s="14"/>
+      <c r="N99" s="14"/>
+      <c r="O99" s="14"/>
+      <c r="P99" s="14"/>
+      <c r="S99" s="14"/>
+      <c r="T99" s="14"/>
+    </row>
+    <row r="100" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M100" s="14"/>
+      <c r="N100" s="14"/>
+      <c r="O100" s="14"/>
+      <c r="P100" s="14"/>
+      <c r="S100" s="14"/>
+      <c r="T100" s="14"/>
+    </row>
+    <row r="101" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M101" s="14"/>
+      <c r="N101" s="14"/>
+      <c r="O101" s="14"/>
+      <c r="P101" s="14"/>
+      <c r="S101" s="14"/>
+      <c r="T101" s="14"/>
+    </row>
+    <row r="102" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M102" s="14"/>
+      <c r="N102" s="14"/>
+      <c r="O102" s="14"/>
+      <c r="P102" s="14"/>
+      <c r="S102" s="14"/>
+      <c r="T102" s="14"/>
+    </row>
+    <row r="103" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M103" s="14"/>
+      <c r="N103" s="14"/>
+      <c r="O103" s="14"/>
+      <c r="P103" s="14"/>
+      <c r="S103" s="14"/>
+      <c r="T103" s="14"/>
+    </row>
+    <row r="104" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M104" s="14"/>
+      <c r="N104" s="14"/>
+      <c r="O104" s="14"/>
+      <c r="P104" s="14"/>
+      <c r="S104" s="14"/>
+      <c r="T104" s="14"/>
+    </row>
+    <row r="105" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M105" s="14"/>
+      <c r="N105" s="14"/>
+      <c r="O105" s="14"/>
+      <c r="P105" s="14"/>
+      <c r="S105" s="14"/>
+      <c r="T105" s="14"/>
+    </row>
+    <row r="106" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M106" s="14"/>
+      <c r="N106" s="14"/>
+      <c r="O106" s="14"/>
+      <c r="P106" s="14"/>
+      <c r="S106" s="14"/>
+      <c r="T106" s="14"/>
+    </row>
+    <row r="107" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M107" s="14"/>
+      <c r="N107" s="14"/>
+      <c r="O107" s="14"/>
+      <c r="P107" s="14"/>
+      <c r="S107" s="14"/>
+      <c r="T107" s="14"/>
+    </row>
+    <row r="108" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M108" s="14"/>
+      <c r="N108" s="14"/>
+      <c r="O108" s="14"/>
+      <c r="P108" s="14"/>
+      <c r="S108" s="14"/>
+      <c r="T108" s="14"/>
+    </row>
+    <row r="109" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M109" s="14"/>
+      <c r="N109" s="14"/>
+      <c r="O109" s="14"/>
+      <c r="P109" s="14"/>
+      <c r="S109" s="14"/>
+      <c r="T109" s="14"/>
+    </row>
+    <row r="110" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M110" s="14"/>
+      <c r="N110" s="14"/>
+      <c r="O110" s="14"/>
+      <c r="P110" s="14"/>
+      <c r="S110" s="14"/>
+      <c r="T110" s="14"/>
+    </row>
+    <row r="111" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M111" s="14"/>
+      <c r="N111" s="14"/>
+      <c r="O111" s="14"/>
+      <c r="P111" s="14"/>
+      <c r="S111" s="14"/>
+      <c r="T111" s="14"/>
+    </row>
+    <row r="112" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M112" s="14"/>
+      <c r="N112" s="14"/>
+      <c r="O112" s="14"/>
+      <c r="P112" s="14"/>
+      <c r="S112" s="14"/>
+      <c r="T112" s="14"/>
+    </row>
+    <row r="113" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M113" s="14"/>
+      <c r="N113" s="14"/>
+      <c r="O113" s="14"/>
+      <c r="P113" s="14"/>
+      <c r="S113" s="14"/>
+      <c r="T113" s="14"/>
+    </row>
+    <row r="114" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M114" s="14"/>
+      <c r="N114" s="14"/>
+      <c r="O114" s="14"/>
+      <c r="P114" s="14"/>
+      <c r="S114" s="14"/>
+      <c r="T114" s="14"/>
+    </row>
+    <row r="115" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M115" s="14"/>
+      <c r="N115" s="14"/>
+      <c r="O115" s="14"/>
+      <c r="P115" s="14"/>
+      <c r="S115" s="14"/>
+      <c r="T115" s="14"/>
+    </row>
+    <row r="116" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M116" s="14"/>
+      <c r="N116" s="14"/>
+      <c r="O116" s="14"/>
+      <c r="P116" s="14"/>
+      <c r="S116" s="14"/>
+      <c r="T116" s="14"/>
+    </row>
+    <row r="117" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M117" s="14"/>
+      <c r="N117" s="14"/>
+      <c r="O117" s="14"/>
+      <c r="P117" s="14"/>
+      <c r="S117" s="14"/>
+      <c r="T117" s="14"/>
+    </row>
+    <row r="118" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M118" s="14"/>
+      <c r="N118" s="14"/>
+      <c r="O118" s="14"/>
+      <c r="P118" s="14"/>
+      <c r="S118" s="14"/>
+      <c r="T118" s="14"/>
+    </row>
+    <row r="119" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M119" s="14"/>
+      <c r="N119" s="14"/>
+      <c r="O119" s="14"/>
+      <c r="P119" s="14"/>
+      <c r="S119" s="14"/>
+      <c r="T119" s="14"/>
+    </row>
+    <row r="120" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M120" s="14"/>
+      <c r="N120" s="14"/>
+      <c r="O120" s="14"/>
+      <c r="P120" s="14"/>
+      <c r="S120" s="14"/>
+      <c r="T120" s="14"/>
+    </row>
+    <row r="121" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M121" s="14"/>
+      <c r="N121" s="14"/>
+      <c r="O121" s="14"/>
+      <c r="P121" s="14"/>
+      <c r="S121" s="14"/>
+      <c r="T121" s="14"/>
+    </row>
+    <row r="122" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M122" s="14"/>
+      <c r="N122" s="14"/>
+      <c r="O122" s="14"/>
+      <c r="P122" s="14"/>
+      <c r="S122" s="14"/>
+      <c r="T122" s="14"/>
+    </row>
+    <row r="123" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M123" s="14"/>
+      <c r="N123" s="14"/>
+      <c r="O123" s="14"/>
+      <c r="P123" s="14"/>
+      <c r="S123" s="14"/>
+      <c r="T123" s="14"/>
+    </row>
+    <row r="124" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M124" s="14"/>
+      <c r="N124" s="14"/>
+      <c r="O124" s="14"/>
+      <c r="P124" s="14"/>
+      <c r="S124" s="14"/>
+      <c r="T124" s="14"/>
+    </row>
+    <row r="125" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M125" s="14"/>
+      <c r="N125" s="14"/>
+      <c r="O125" s="14"/>
+      <c r="P125" s="14"/>
+      <c r="S125" s="14"/>
+      <c r="T125" s="14"/>
+    </row>
+    <row r="126" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M126" s="14"/>
+      <c r="N126" s="14"/>
+      <c r="O126" s="14"/>
+      <c r="P126" s="14"/>
+      <c r="S126" s="14"/>
+      <c r="T126" s="14"/>
+    </row>
+    <row r="127" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M127" s="14"/>
+      <c r="N127" s="14"/>
+      <c r="O127" s="14"/>
+      <c r="P127" s="14"/>
+      <c r="S127" s="14"/>
+      <c r="T127" s="14"/>
+    </row>
+    <row r="128" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M128" s="14"/>
+      <c r="N128" s="14"/>
+      <c r="O128" s="14"/>
+      <c r="P128" s="14"/>
+      <c r="S128" s="14"/>
+      <c r="T128" s="14"/>
+    </row>
+    <row r="129" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M129" s="14"/>
+      <c r="N129" s="14"/>
+      <c r="O129" s="14"/>
+      <c r="P129" s="14"/>
+      <c r="S129" s="14"/>
+      <c r="T129" s="14"/>
+    </row>
+    <row r="130" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M130" s="14"/>
+      <c r="N130" s="14"/>
+      <c r="O130" s="14"/>
+      <c r="P130" s="14"/>
+    </row>
+    <row r="131" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M131" s="14"/>
+      <c r="N131" s="14"/>
+      <c r="O131" s="14"/>
+      <c r="P131" s="14"/>
+    </row>
+    <row r="132" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M132" s="14"/>
+      <c r="N132" s="14"/>
+      <c r="O132" s="14"/>
+      <c r="P132" s="14"/>
+    </row>
+    <row r="133" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M133" s="14"/>
+      <c r="N133" s="14"/>
+      <c r="O133" s="14"/>
+      <c r="P133" s="14"/>
+    </row>
+    <row r="134" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M134" s="14"/>
+      <c r="N134" s="14"/>
+      <c r="O134" s="14"/>
+      <c r="P134" s="14"/>
+    </row>
+    <row r="135" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M135" s="14"/>
+      <c r="N135" s="14"/>
+      <c r="O135" s="14"/>
+      <c r="P135" s="14"/>
+    </row>
+    <row r="136" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M136" s="14"/>
+      <c r="N136" s="14"/>
+      <c r="O136" s="14"/>
+      <c r="P136" s="14"/>
+    </row>
+    <row r="137" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M137" s="14"/>
+      <c r="N137" s="14"/>
+      <c r="O137" s="14"/>
+      <c r="P137" s="14"/>
+    </row>
+    <row r="138" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M138" s="14"/>
+      <c r="N138" s="14"/>
+      <c r="O138" s="14"/>
+      <c r="P138" s="14"/>
+    </row>
+    <row r="139" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M139" s="14"/>
+      <c r="N139" s="14"/>
+      <c r="O139" s="14"/>
+      <c r="P139" s="14"/>
+    </row>
+    <row r="140" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M140" s="14"/>
+      <c r="N140" s="14"/>
+      <c r="O140" s="14"/>
+      <c r="P140" s="14"/>
+    </row>
+    <row r="141" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M141" s="14"/>
+      <c r="N141" s="14"/>
+      <c r="O141" s="14"/>
+      <c r="P141" s="14"/>
+    </row>
+    <row r="142" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M142" s="14"/>
+      <c r="N142" s="14"/>
+      <c r="O142" s="14"/>
+      <c r="P142" s="14"/>
+    </row>
+    <row r="143" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M143" s="14"/>
+      <c r="N143" s="14"/>
+      <c r="O143" s="14"/>
+      <c r="P143" s="14"/>
+    </row>
+    <row r="144" spans="13:20" x14ac:dyDescent="0.3">
+      <c r="M144" s="14"/>
+      <c r="N144" s="14"/>
+      <c r="O144" s="14"/>
+      <c r="P144" s="14"/>
+    </row>
+    <row r="145" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M145" s="14"/>
+      <c r="N145" s="14"/>
+      <c r="O145" s="14"/>
+      <c r="P145" s="14"/>
+    </row>
+    <row r="146" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M146" s="14"/>
+      <c r="N146" s="14"/>
+      <c r="O146" s="14"/>
+      <c r="P146" s="14"/>
+    </row>
+    <row r="147" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M147" s="14"/>
+      <c r="N147" s="14"/>
+      <c r="O147" s="14"/>
+      <c r="P147" s="14"/>
+    </row>
+    <row r="148" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M148" s="14"/>
+      <c r="N148" s="14"/>
+      <c r="O148" s="14"/>
+      <c r="P148" s="14"/>
+    </row>
+    <row r="149" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M149" s="14"/>
+      <c r="N149" s="14"/>
+      <c r="O149" s="14"/>
+      <c r="P149" s="14"/>
+    </row>
+    <row r="150" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M150" s="14"/>
+      <c r="N150" s="14"/>
+      <c r="O150" s="14"/>
+      <c r="P150" s="14"/>
+    </row>
+    <row r="151" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M151" s="14"/>
+      <c r="N151" s="14"/>
+      <c r="O151" s="14"/>
+      <c r="P151" s="14"/>
+    </row>
+    <row r="152" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M152" s="14"/>
+      <c r="N152" s="14"/>
+      <c r="O152" s="14"/>
+      <c r="P152" s="14"/>
+    </row>
+    <row r="153" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M153" s="14"/>
+      <c r="N153" s="14"/>
+      <c r="O153" s="14"/>
+      <c r="P153" s="14"/>
+    </row>
+    <row r="154" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M154" s="14"/>
+      <c r="N154" s="14"/>
+      <c r="O154" s="14"/>
+      <c r="P154" s="14"/>
+    </row>
+    <row r="155" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M155" s="14"/>
+      <c r="N155" s="14"/>
+      <c r="O155" s="14"/>
+      <c r="P155" s="14"/>
+    </row>
+    <row r="156" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M156" s="14"/>
+      <c r="N156" s="14"/>
+      <c r="O156" s="14"/>
+      <c r="P156" s="14"/>
+    </row>
+    <row r="157" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M157" s="14"/>
+      <c r="N157" s="14"/>
+      <c r="O157" s="14"/>
+      <c r="P157" s="14"/>
+    </row>
+    <row r="158" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M158" s="14"/>
+      <c r="N158" s="14"/>
+      <c r="O158" s="14"/>
+      <c r="P158" s="14"/>
+    </row>
+    <row r="159" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M159" s="14"/>
+      <c r="N159" s="14"/>
+      <c r="O159" s="14"/>
+      <c r="P159" s="14"/>
+    </row>
+    <row r="160" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M160" s="14"/>
+      <c r="N160" s="14"/>
+      <c r="O160" s="14"/>
+      <c r="P160" s="14"/>
+    </row>
+    <row r="161" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M161" s="14"/>
+      <c r="N161" s="14"/>
+      <c r="O161" s="14"/>
+      <c r="P161" s="14"/>
+    </row>
+    <row r="162" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M162" s="14"/>
+      <c r="N162" s="14"/>
+      <c r="O162" s="14"/>
+      <c r="P162" s="14"/>
+    </row>
+    <row r="163" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M163" s="14"/>
+      <c r="N163" s="14"/>
+      <c r="O163" s="14"/>
+      <c r="P163" s="14"/>
+    </row>
+    <row r="164" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M164" s="14"/>
+      <c r="N164" s="14"/>
+      <c r="O164" s="14"/>
+      <c r="P164" s="14"/>
+    </row>
+    <row r="165" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M165" s="14"/>
+      <c r="N165" s="14"/>
+      <c r="O165" s="14"/>
+      <c r="P165" s="14"/>
+    </row>
+    <row r="166" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M166" s="14"/>
+      <c r="N166" s="14"/>
+      <c r="O166" s="14"/>
+      <c r="P166" s="14"/>
+    </row>
+    <row r="167" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M167" s="14"/>
+      <c r="N167" s="14"/>
+      <c r="O167" s="14"/>
+      <c r="P167" s="14"/>
+    </row>
+    <row r="168" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M168" s="14"/>
+      <c r="N168" s="14"/>
+      <c r="O168" s="14"/>
+      <c r="P168" s="14"/>
+    </row>
+    <row r="169" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M169" s="14"/>
+      <c r="N169" s="14"/>
+      <c r="O169" s="14"/>
+      <c r="P169" s="14"/>
+    </row>
+    <row r="170" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M170" s="14"/>
+      <c r="N170" s="14"/>
+      <c r="O170" s="14"/>
+      <c r="P170" s="14"/>
+    </row>
+    <row r="171" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M171" s="14"/>
+      <c r="N171" s="14"/>
+      <c r="O171" s="14"/>
+      <c r="P171" s="14"/>
+    </row>
+    <row r="172" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M172" s="14"/>
+      <c r="N172" s="14"/>
+      <c r="O172" s="14"/>
+      <c r="P172" s="14"/>
+    </row>
+    <row r="173" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M173" s="14"/>
+      <c r="N173" s="14"/>
+      <c r="O173" s="14"/>
+      <c r="P173" s="14"/>
+    </row>
+    <row r="174" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M174" s="14"/>
+      <c r="N174" s="14"/>
+      <c r="O174" s="14"/>
+      <c r="P174" s="14"/>
+    </row>
+    <row r="175" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M175" s="14"/>
+      <c r="N175" s="14"/>
+      <c r="O175" s="14"/>
+      <c r="P175" s="14"/>
+    </row>
+    <row r="176" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M176" s="14"/>
+      <c r="N176" s="14"/>
+      <c r="O176" s="14"/>
+      <c r="P176" s="14"/>
+    </row>
+    <row r="177" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M177" s="14"/>
+      <c r="N177" s="14"/>
+      <c r="O177" s="14"/>
+      <c r="P177" s="14"/>
+    </row>
+    <row r="178" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M178" s="14"/>
+      <c r="N178" s="14"/>
+      <c r="O178" s="14"/>
+      <c r="P178" s="14"/>
+    </row>
+    <row r="179" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M179" s="14"/>
+      <c r="N179" s="14"/>
+      <c r="O179" s="14"/>
+      <c r="P179" s="14"/>
+    </row>
+    <row r="180" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M180" s="14"/>
+      <c r="N180" s="14"/>
+      <c r="O180" s="14"/>
+      <c r="P180" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -754,67 +2459,40 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23AEAE26-C3F0-4F31-AF0B-F3D56F91F681}">
-  <dimension ref="A21:A64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A4256-682D-4383-AE0D-B380D1080FD1}">
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.25" customWidth="1"/>
-    <col min="4" max="4" width="32.08203125" customWidth="1"/>
-    <col min="6" max="6" width="10.75" customWidth="1"/>
+    <col min="1" max="1" width="17.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="4" t="s">
-        <v>14</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E61">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="1" tint="0.14999847407452621"/>
-        <color rgb="FFBFB93F"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Since I didn't finish tasks promptly and well, I resceduled tasks in design phase.
</commit_message>
<xml_diff>
--- a/MainAgenda.xlsx
+++ b/MainAgenda.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D4DF1E09-830E-4307-8BF1-3B6613F472A2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0E38FE2D-C21C-4B87-8E78-04BCE0E24239}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,6 +11,7 @@
     <sheet name="总体计划草图" sheetId="1" r:id="rId1"/>
     <sheet name="V0.1.0开发计划" sheetId="3" r:id="rId2"/>
     <sheet name="交付物" sheetId="4" r:id="rId3"/>
+    <sheet name="修订日志" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -193,6 +194,22 @@
   </si>
   <si>
     <t>界面原型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V0.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始版本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周末没有按时完成任务，调整设计阶段的安排</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -200,7 +217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,8 +268,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,8 +317,14 @@
         <fgColor theme="6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -319,8 +350,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -334,8 +374,11 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -357,8 +400,14 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="3" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="5" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="5" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="3" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="40% - 着色 5" xfId="5" builtinId="47"/>
     <cellStyle name="标题 2" xfId="1" builtinId="17"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="着色 2" xfId="2" builtinId="33"/>
@@ -369,10 +418,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF0000"/>
       <color rgb="FFBFB93F"/>
       <color rgb="FFD6CC0C"/>
       <color rgb="FFCD6969"/>
-      <color rgb="FFFF0000"/>
     </mruColors>
   </colors>
   <extLst>
@@ -731,13 +780,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC988E25-B343-4608-AF8D-463AF7A5B44B}">
-  <dimension ref="A1:Y180"/>
+  <dimension ref="A1:AB180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B7" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -749,7 +798,7 @@
     <col min="25" max="25" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -826,12 +875,13 @@
         <v>43222</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P2" s="21"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -844,415 +894,368 @@
       <c r="H3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="14"/>
-      <c r="O3" s="17" t="s">
+      <c r="P3" s="21"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="S3" s="14"/>
-      <c r="W3" s="18" t="s">
+      <c r="V3" s="14"/>
+      <c r="Z3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="Y3" s="18" t="s">
+      <c r="AB3" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="7"/>
       <c r="H4" s="10"/>
-      <c r="I4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="10"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="W4" s="10"/>
-      <c r="Y4" s="10"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="L4" s="14"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="10"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="Z4" s="10"/>
+      <c r="AB4" s="10"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="H5" s="10"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="10"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="W5" s="10"/>
-      <c r="Y5" s="10"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P5" s="21"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="10"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="Z5" s="10"/>
+      <c r="AB5" s="10"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="7"/>
       <c r="H6" s="10"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="10"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="W6" s="10"/>
-      <c r="Y6" s="10"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P6" s="21"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="10"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="Z6" s="10"/>
+      <c r="AB6" s="10"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="7"/>
       <c r="H7" s="10"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="10"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="W7" s="10"/>
-      <c r="Y7" s="10"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P7" s="21"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="10"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="14"/>
+      <c r="Z7" s="10"/>
+      <c r="AB7" s="10"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="7"/>
       <c r="H8" s="10"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="10"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="W8" s="10"/>
-      <c r="Y8" s="10"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P8" s="21"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="10"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="Z8" s="10"/>
+      <c r="AB8" s="10"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="7"/>
       <c r="H9" s="10"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="10"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="W9" s="10"/>
-      <c r="Y9" s="10"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P9" s="21"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="10"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="Z9" s="10"/>
+      <c r="AB9" s="10"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="7"/>
       <c r="H10" s="10"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="10"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="W10" s="10"/>
-      <c r="Y10" s="10"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P10" s="21"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="10"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
+      <c r="Z10" s="10"/>
+      <c r="AB10" s="10"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="9"/>
       <c r="H11" s="10"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="10"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="W11" s="10"/>
-      <c r="Y11" s="10"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="I11" s="19"/>
+      <c r="K11" s="10"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="10"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="Z11" s="10"/>
+      <c r="AB11" s="10"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="11"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="10"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="W12" s="10"/>
-      <c r="Y12" s="10"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="G12" s="9"/>
+      <c r="H12" s="12"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="20"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="10"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="Z12" s="10"/>
+      <c r="AB12" s="10"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
       <c r="H13" s="10"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
       <c r="L13" s="9"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="10"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="W13" s="10"/>
-      <c r="Y13" s="10"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="22"/>
+      <c r="R13" s="10"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="14"/>
+      <c r="Z13" s="10"/>
+      <c r="AB13" s="10"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H14" s="10"/>
-      <c r="I14" s="8"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="14"/>
+      <c r="L14" s="8"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="10"/>
       <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="W14" s="10"/>
-      <c r="Y14" s="10"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="Z14" s="10"/>
+      <c r="AB14" s="10"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H15" s="10"/>
-      <c r="J15" s="8"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="14"/>
+      <c r="L15" s="8"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="10"/>
       <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="14"/>
-      <c r="W15" s="10"/>
-      <c r="Y15" s="10"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
+      <c r="Z15" s="10"/>
+      <c r="AB15" s="10"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H16" s="10"/>
-      <c r="K16" s="8"/>
       <c r="L16" s="8"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="14"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="10"/>
       <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="W16" s="10"/>
-      <c r="Y16" s="10"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V16" s="14"/>
+      <c r="W16" s="14"/>
+      <c r="Z16" s="10"/>
+      <c r="AB16" s="10"/>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
       <c r="H17" s="10"/>
-      <c r="M17" s="8"/>
+      <c r="M17" s="16"/>
       <c r="N17" s="16"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="14"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="21"/>
       <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
-      <c r="W17" s="10"/>
-      <c r="Y17" s="10"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V17" s="14"/>
+      <c r="W17" s="14"/>
+      <c r="Z17" s="10"/>
+      <c r="AB17" s="10"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H18" s="10"/>
+      <c r="M18" s="14"/>
       <c r="N18" s="16"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="14"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="23"/>
       <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="W18" s="10"/>
-      <c r="Y18" s="10"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V18" s="14"/>
+      <c r="W18" s="14"/>
+      <c r="Z18" s="10"/>
+      <c r="AB18" s="10"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="H19" s="10"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="9"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="10"/>
       <c r="S19" s="9"/>
       <c r="T19" s="15"/>
-      <c r="U19" s="15"/>
-      <c r="V19" s="15"/>
-      <c r="W19" s="12"/>
-      <c r="Y19" s="10"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="15"/>
+      <c r="Z19" s="12"/>
+      <c r="AB19" s="10"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H20" s="10"/>
-      <c r="M20" s="14"/>
       <c r="N20" s="14"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
-      <c r="W20" s="10"/>
-      <c r="Y20" s="10"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P20" s="21"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="W20" s="14"/>
+      <c r="X20" s="14"/>
+      <c r="Z20" s="10"/>
+      <c r="AB20" s="10"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>37</v>
       </c>
       <c r="H21" s="10"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="10"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="16"/>
-      <c r="U21" s="14"/>
-      <c r="W21" s="10"/>
-      <c r="Y21" s="10"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P21" s="21"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="10"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="16"/>
+      <c r="X21" s="14"/>
+      <c r="Z21" s="10"/>
+      <c r="AB21" s="10"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>40</v>
       </c>
       <c r="H22" s="10"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="10"/>
-      <c r="T22" s="16"/>
-      <c r="U22" s="14"/>
-      <c r="W22" s="10"/>
-      <c r="Y22" s="10"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P22" s="21"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="10"/>
+      <c r="W22" s="16"/>
+      <c r="X22" s="14"/>
+      <c r="Z22" s="10"/>
+      <c r="AB22" s="10"/>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>39</v>
       </c>
       <c r="H23" s="10"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="10"/>
-      <c r="T23" s="14"/>
-      <c r="U23" s="16"/>
-      <c r="V23" s="8"/>
-      <c r="W23" s="11"/>
-      <c r="Y23" s="10"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="L23" s="14"/>
+      <c r="P23" s="21"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="10"/>
+      <c r="W23" s="14"/>
+      <c r="X23" s="16"/>
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="11"/>
+      <c r="AB23" s="10"/>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>40</v>
       </c>
       <c r="H24" s="10"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="10"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="14"/>
-      <c r="W24" s="11"/>
-      <c r="Y24" s="10"/>
-    </row>
-    <row r="25" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P24" s="21"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="10"/>
+      <c r="W24" s="14"/>
+      <c r="X24" s="14"/>
+      <c r="Z24" s="11"/>
+      <c r="AB24" s="10"/>
+    </row>
+    <row r="25" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>30</v>
       </c>
       <c r="H25" s="10"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="10"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="14"/>
-      <c r="W25" s="10"/>
-      <c r="X25" s="9"/>
-      <c r="Y25" s="12"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="P25" s="21"/>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="10"/>
+      <c r="W25" s="14"/>
+      <c r="X25" s="14"/>
+      <c r="Z25" s="10"/>
+      <c r="AA25" s="9"/>
+      <c r="AB25" s="12"/>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H26" s="10"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="10"/>
       <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="T26" s="14"/>
-      <c r="U26" s="14"/>
-      <c r="W26" s="10"/>
-      <c r="Y26" s="10"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H27" s="10"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="14"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
-      <c r="W27" s="10"/>
-      <c r="Y27" s="10"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H28" s="10"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="14"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="14"/>
-      <c r="W28" s="10"/>
-      <c r="Y28" s="10"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H29" s="10"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="14"/>
-      <c r="S29" s="14"/>
-      <c r="T29" s="14"/>
-      <c r="W29" s="10"/>
-      <c r="Y29" s="10"/>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H30" s="10"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="14"/>
-      <c r="S30" s="14"/>
-      <c r="T30" s="14"/>
-      <c r="W30" s="10"/>
-      <c r="Y30" s="10"/>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H31" s="10"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="14"/>
-      <c r="S31" s="14"/>
-      <c r="T31" s="14"/>
-      <c r="W31" s="10"/>
-      <c r="Y31" s="10"/>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H32" s="10"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="14"/>
-      <c r="S32" s="14"/>
-      <c r="T32" s="14"/>
-      <c r="W32" s="10"/>
-      <c r="Y32" s="10"/>
     </row>
     <row r="33" spans="8:25" x14ac:dyDescent="0.3">
       <c r="H33" s="10"/>
@@ -2495,4 +2498,39 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37FAB6B8-92CD-4261-907E-D9F2D8D85A7E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="42.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>